<commit_message>
Test the UI form separated according to kinds of arts
</commit_message>
<xml_diff>
--- a/data/FrameData_Read.xlsx
+++ b/data/FrameData_Read.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\program\flutter_projct\combo_maker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD2C4DD-17EA-4E43-9A43-7B5D1D89786D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4876F9C-A2A6-4C2C-B1ED-89143CE5083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{29058C92-C9D0-46B6-BABB-3C4B733B9124}"/>
   </bookViews>
@@ -5334,15 +5334,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA8BD0E-4BBD-41B5-BE09-A17217706007}">
-  <dimension ref="A1:T63"/>
+  <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="V46" sqref="V46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>201</v>
       </c>
@@ -5400,11 +5400,14 @@
       <c r="S1" t="s">
         <v>3</v>
       </c>
-      <c r="T1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="T1">
+        <v>0</v>
+      </c>
+      <c r="U1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -5462,11 +5465,14 @@
       <c r="S2" t="s">
         <v>3</v>
       </c>
-      <c r="T2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -5524,11 +5530,14 @@
       <c r="S3" t="s">
         <v>3</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -5586,11 +5595,14 @@
       <c r="S4" t="s">
         <v>3</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>209</v>
       </c>
@@ -5648,11 +5660,14 @@
       <c r="S5" t="s">
         <v>3</v>
       </c>
-      <c r="T5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -5710,11 +5725,14 @@
       <c r="S6" t="s">
         <v>3</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>2</v>
       </c>
@@ -5772,11 +5790,14 @@
       <c r="S7" t="s">
         <v>3</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>2</v>
       </c>
@@ -5834,11 +5855,14 @@
       <c r="S8" t="s">
         <v>15</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>2</v>
       </c>
@@ -5896,11 +5920,14 @@
       <c r="S9" t="s">
         <v>3</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>2</v>
       </c>
@@ -5958,11 +5985,14 @@
       <c r="S10" t="s">
         <v>15</v>
       </c>
-      <c r="T10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>2</v>
       </c>
@@ -6020,11 +6050,14 @@
       <c r="S11" t="s">
         <v>15</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>2</v>
       </c>
@@ -6082,16 +6115,19 @@
       <c r="S12" t="s">
         <v>3</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C13" t="s">
         <v>202</v>
@@ -6144,16 +6180,19 @@
       <c r="S13" t="s">
         <v>6</v>
       </c>
-      <c r="T13" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
         <v>202</v>
@@ -6206,16 +6245,19 @@
       <c r="S14" t="s">
         <v>6</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="B15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C15" t="s">
         <v>202</v>
@@ -6268,16 +6310,19 @@
       <c r="S15" t="s">
         <v>6</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="C16" t="s">
         <v>202</v>
@@ -6330,16 +6375,19 @@
       <c r="S16" t="s">
         <v>6</v>
       </c>
-      <c r="T16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
         <v>202</v>
@@ -6392,16 +6440,19 @@
       <c r="S17" t="s">
         <v>6</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
         <v>202</v>
@@ -6454,11 +6505,14 @@
       <c r="S18" t="s">
         <v>6</v>
       </c>
-      <c r="T18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>224</v>
       </c>
@@ -6516,11 +6570,14 @@
       <c r="S19" t="s">
         <v>6</v>
       </c>
-      <c r="T19" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>225</v>
       </c>
@@ -6578,11 +6635,14 @@
       <c r="S20" t="s">
         <v>3</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>225</v>
       </c>
@@ -6640,19 +6700,22 @@
       <c r="S21" t="s">
         <v>3</v>
       </c>
-      <c r="T21" t="s">
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D22" t="s">
         <v>202</v>
@@ -6702,11 +6765,14 @@
       <c r="S22" t="s">
         <v>6</v>
       </c>
-      <c r="T22" t="s">
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>201</v>
       </c>
@@ -6764,11 +6830,14 @@
       <c r="S23" t="s">
         <v>3</v>
       </c>
-      <c r="T23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>209</v>
       </c>
@@ -6826,11 +6895,14 @@
       <c r="S24" t="s">
         <v>3</v>
       </c>
-      <c r="T24" t="s">
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>229</v>
       </c>
@@ -6885,11 +6957,14 @@
       <c r="S25" t="s">
         <v>54</v>
       </c>
-      <c r="T25" t="s">
+      <c r="T25">
+        <v>2</v>
+      </c>
+      <c r="U25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>229</v>
       </c>
@@ -6947,11 +7022,14 @@
       <c r="S26" t="s">
         <v>3</v>
       </c>
-      <c r="T26" t="s">
+      <c r="T26">
+        <v>2</v>
+      </c>
+      <c r="U26" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>229</v>
       </c>
@@ -7006,11 +7084,14 @@
       <c r="S27" t="s">
         <v>54</v>
       </c>
-      <c r="T27" t="s">
+      <c r="T27">
+        <v>2</v>
+      </c>
+      <c r="U27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -7068,11 +7149,14 @@
       <c r="S28" t="s">
         <v>3</v>
       </c>
-      <c r="T28" t="s">
+      <c r="T28">
+        <v>2</v>
+      </c>
+      <c r="U28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>229</v>
       </c>
@@ -7130,11 +7214,14 @@
       <c r="S29" t="s">
         <v>54</v>
       </c>
-      <c r="T29" t="s">
+      <c r="T29">
+        <v>2</v>
+      </c>
+      <c r="U29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>229</v>
       </c>
@@ -7192,11 +7279,14 @@
       <c r="S30" t="s">
         <v>54</v>
       </c>
-      <c r="T30" t="s">
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="U30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>229</v>
       </c>
@@ -7254,11 +7344,14 @@
       <c r="S31" t="s">
         <v>202</v>
       </c>
-      <c r="T31" t="s">
+      <c r="T31">
+        <v>2</v>
+      </c>
+      <c r="U31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>229</v>
       </c>
@@ -7316,11 +7409,14 @@
       <c r="S32" t="s">
         <v>3</v>
       </c>
-      <c r="T32" t="s">
+      <c r="T32">
+        <v>2</v>
+      </c>
+      <c r="U32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>185</v>
       </c>
@@ -7378,11 +7474,14 @@
       <c r="S33" t="s">
         <v>3</v>
       </c>
-      <c r="T33" t="s">
+      <c r="T33">
+        <v>2</v>
+      </c>
+      <c r="U33" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -7440,11 +7539,14 @@
       <c r="S34" t="s">
         <v>3</v>
       </c>
-      <c r="T34" t="s">
+      <c r="T34">
+        <v>2</v>
+      </c>
+      <c r="U34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
         <v>185</v>
       </c>
@@ -7502,11 +7604,14 @@
       <c r="S35" t="s">
         <v>3</v>
       </c>
-      <c r="T35" t="s">
+      <c r="T35">
+        <v>2</v>
+      </c>
+      <c r="U35" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -7564,11 +7669,14 @@
       <c r="S36" t="s">
         <v>3</v>
       </c>
-      <c r="T36" t="s">
+      <c r="T36">
+        <v>2</v>
+      </c>
+      <c r="U36" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>229</v>
       </c>
@@ -7626,11 +7734,14 @@
       <c r="S37" t="s">
         <v>3</v>
       </c>
-      <c r="T37" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="T37">
+        <v>2</v>
+      </c>
+      <c r="U37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
         <v>229</v>
       </c>
@@ -7688,11 +7799,14 @@
       <c r="S38" t="s">
         <v>3</v>
       </c>
-      <c r="T38" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="T38">
+        <v>2</v>
+      </c>
+      <c r="U38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
         <v>229</v>
       </c>
@@ -7750,11 +7864,14 @@
       <c r="S39" t="s">
         <v>3</v>
       </c>
-      <c r="T39" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20">
+      <c r="T39">
+        <v>2</v>
+      </c>
+      <c r="U39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
         <v>229</v>
       </c>
@@ -7812,11 +7929,14 @@
       <c r="S40" t="s">
         <v>3</v>
       </c>
-      <c r="T40" t="s">
+      <c r="T40">
+        <v>2</v>
+      </c>
+      <c r="U40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -7874,11 +7994,14 @@
       <c r="S41" t="s">
         <v>202</v>
       </c>
-      <c r="T41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20">
+      <c r="T41">
+        <v>2</v>
+      </c>
+      <c r="U41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
         <v>185</v>
       </c>
@@ -7936,11 +8059,14 @@
       <c r="S42" t="s">
         <v>202</v>
       </c>
-      <c r="T42" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="T42">
+        <v>2</v>
+      </c>
+      <c r="U42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
         <v>185</v>
       </c>
@@ -7998,11 +8124,14 @@
       <c r="S43" t="s">
         <v>202</v>
       </c>
-      <c r="T43" t="s">
+      <c r="T43">
+        <v>2</v>
+      </c>
+      <c r="U43" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
         <v>185</v>
       </c>
@@ -8060,11 +8189,14 @@
       <c r="S44" t="s">
         <v>202</v>
       </c>
-      <c r="T44" t="s">
+      <c r="T44">
+        <v>2</v>
+      </c>
+      <c r="U44" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
         <v>226</v>
       </c>
@@ -8122,11 +8254,14 @@
       <c r="S45" t="s">
         <v>202</v>
       </c>
-      <c r="T45" t="s">
+      <c r="T45">
+        <v>2</v>
+      </c>
+      <c r="U45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
         <v>226</v>
       </c>
@@ -8184,11 +8319,14 @@
       <c r="S46" t="s">
         <v>3</v>
       </c>
-      <c r="T46" t="s">
+      <c r="T46">
+        <v>2</v>
+      </c>
+      <c r="U46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
         <v>226</v>
       </c>
@@ -8246,11 +8384,14 @@
       <c r="S47" t="s">
         <v>3</v>
       </c>
-      <c r="T47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20">
+      <c r="T47">
+        <v>2</v>
+      </c>
+      <c r="U47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>226</v>
       </c>
@@ -8308,11 +8449,14 @@
       <c r="S48" t="s">
         <v>111</v>
       </c>
-      <c r="T48" t="s">
+      <c r="T48">
+        <v>2</v>
+      </c>
+      <c r="U48" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:21">
       <c r="A49" t="s">
         <v>235</v>
       </c>
@@ -8370,11 +8514,14 @@
       <c r="S49" t="s">
         <v>3</v>
       </c>
-      <c r="T49" t="s">
+      <c r="T49">
+        <v>3</v>
+      </c>
+      <c r="U49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:21">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -8432,11 +8579,14 @@
       <c r="S50" t="s">
         <v>54</v>
       </c>
-      <c r="T50" t="s">
+      <c r="T50">
+        <v>3</v>
+      </c>
+      <c r="U50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:21">
       <c r="A51" t="s">
         <v>235</v>
       </c>
@@ -8494,11 +8644,14 @@
       <c r="S51" t="s">
         <v>3</v>
       </c>
-      <c r="T51" t="s">
+      <c r="T51">
+        <v>3</v>
+      </c>
+      <c r="U51" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:21">
       <c r="A52" t="s">
         <v>235</v>
       </c>
@@ -8556,11 +8709,14 @@
       <c r="S52" t="s">
         <v>3</v>
       </c>
-      <c r="T52" t="s">
+      <c r="T52">
+        <v>3</v>
+      </c>
+      <c r="U52" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:21">
       <c r="A53" t="s">
         <v>237</v>
       </c>
@@ -8618,11 +8774,14 @@
       <c r="S53" t="s">
         <v>111</v>
       </c>
-      <c r="T53" t="s">
+      <c r="T53">
+        <v>4</v>
+      </c>
+      <c r="U53" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:21">
       <c r="A54" t="s">
         <v>238</v>
       </c>
@@ -8680,11 +8839,14 @@
       <c r="S54" t="s">
         <v>111</v>
       </c>
-      <c r="T54" t="s">
+      <c r="T54">
+        <v>4</v>
+      </c>
+      <c r="U54" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:21">
       <c r="A55" t="s">
         <v>239</v>
       </c>
@@ -8742,11 +8904,14 @@
       <c r="S55" t="s">
         <v>202</v>
       </c>
-      <c r="T55" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20">
+      <c r="T55">
+        <v>4</v>
+      </c>
+      <c r="U55" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
       <c r="A56" t="s">
         <v>240</v>
       </c>
@@ -8801,11 +8966,14 @@
       <c r="R56">
         <v>0</v>
       </c>
-      <c r="T56" t="s">
+      <c r="T56">
+        <v>4</v>
+      </c>
+      <c r="U56" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:21">
       <c r="A57" t="s">
         <v>241</v>
       </c>
@@ -8863,11 +9031,14 @@
       <c r="S57" t="s">
         <v>3</v>
       </c>
-      <c r="T57" t="s">
+      <c r="T57">
+        <v>4</v>
+      </c>
+      <c r="U57" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:21">
       <c r="A58" t="s">
         <v>225</v>
       </c>
@@ -8925,11 +9096,14 @@
       <c r="S58" t="s">
         <v>3</v>
       </c>
-      <c r="T58" t="s">
+      <c r="T58">
+        <v>4</v>
+      </c>
+      <c r="U58" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:21">
       <c r="A59" t="s">
         <v>242</v>
       </c>
@@ -8987,11 +9161,14 @@
       <c r="S59" t="s">
         <v>202</v>
       </c>
-      <c r="T59" t="s">
+      <c r="T59">
+        <v>4</v>
+      </c>
+      <c r="U59" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:21">
       <c r="A60" t="s">
         <v>242</v>
       </c>
@@ -9049,11 +9226,14 @@
       <c r="S60" t="s">
         <v>202</v>
       </c>
-      <c r="T60" t="s">
+      <c r="T60">
+        <v>4</v>
+      </c>
+      <c r="U60" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:21">
       <c r="A61" t="s">
         <v>242</v>
       </c>
@@ -9111,11 +9291,14 @@
       <c r="S61" t="s">
         <v>202</v>
       </c>
-      <c r="T61" t="s">
+      <c r="T61">
+        <v>4</v>
+      </c>
+      <c r="U61" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:21">
       <c r="A62" t="s">
         <v>242</v>
       </c>
@@ -9173,11 +9356,14 @@
       <c r="S62" t="s">
         <v>202</v>
       </c>
-      <c r="T62" t="s">
+      <c r="T62">
+        <v>4</v>
+      </c>
+      <c r="U62" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:21">
       <c r="A63" t="s">
         <v>202</v>
       </c>
@@ -9235,7 +9421,10 @@
       <c r="S63" t="s">
         <v>202</v>
       </c>
-      <c r="T63" t="s">
+      <c r="T63">
+        <v>4</v>
+      </c>
+      <c r="U63" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>